<commit_message>
#CRM-1615 Add Remarks in SF pending booking page
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
+++ b/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FEB5DC-3E51-4CE5-94F3-A1BA8AE1F86E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C48C3F-FF96-486D-B760-E004766B0837}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Customer Name</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>{bookings:internal_status}</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>{bookings:booking_remarks}</t>
   </si>
 </sst>
 </file>
@@ -488,26 +494,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="2" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="8" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -556,8 +562,11 @@
       <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -605,6 +614,9 @@
       </c>
       <c r="P2" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRM-3026 Add status on download pending booking list on SF CRM
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
+++ b/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C48C3F-FF96-486D-B760-E004766B0837}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A322CC-71E9-47A1-8B54-7C32D9E48B47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Customer Name</t>
   </si>
@@ -109,9 +109,6 @@
     <t>{bookings:booking_alternate_contact_no}</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>{bookings:internal_status}</t>
   </si>
   <si>
@@ -119,13 +116,22 @@
   </si>
   <si>
     <t>{bookings:booking_remarks}</t>
+  </si>
+  <si>
+    <t>Internal Status</t>
+  </si>
+  <si>
+    <t>Current Status</t>
+  </si>
+  <si>
+    <t>{bookings:current_status}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -141,6 +147,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,6 +198,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,129 +518,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="8" width="20.5546875" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" customWidth="1"/>
-    <col min="13" max="13" width="19.88671875" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="9" width="20.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRM-3029 CRM-3024 Add engineer from pending page and auto refresh it also Remove bug of servicible bom and its header issue
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
+++ b/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A322CC-71E9-47A1-8B54-7C32D9E48B47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186113AB-DDBC-41E2-8FFB-052084A681A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Customer Name</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>{bookings:current_status}</t>
+  </si>
+  <si>
+    <t>Engineer Name</t>
+  </si>
+  <si>
+    <t>{bookings:eng_name}</t>
   </si>
 </sst>
 </file>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -533,14 +539,17 @@
     <col min="6" max="7" width="17.44140625" customWidth="1"/>
     <col min="8" max="9" width="20.5546875" customWidth="1"/>
     <col min="10" max="10" width="15.88671875" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
-    <col min="14" max="14" width="19.88671875" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" customWidth="1"/>
-    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="37.109375" customWidth="1"/>
+    <col min="13" max="13" width="24.44140625" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.88671875" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" customWidth="1"/>
+    <col min="17" max="17" width="19.109375" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
@@ -575,28 +584,31 @@
         <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
@@ -631,24 +643,27 @@
         <v>11</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add date limit 30 for review graph and reaarange the excel column
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
+++ b/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186113AB-DDBC-41E2-8FFB-052084A681A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9DCCB2-1B1E-4A53-9321-62997582A8A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,80 +526,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="9" width="20.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="37.109375" customWidth="1"/>
-    <col min="13" max="13" width="24.44140625" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.88671875" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" customWidth="1"/>
+    <col min="12" max="12" width="34.5546875" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="15" max="15" width="24.44140625" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.88671875" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>32</v>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>9</v>
@@ -609,56 +611,56 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>29</v>
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="M2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
CRMS-2360 add create date column tommorow also
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
+++ b/application/controllers/excel-templates/SF-Pending-Bookings-List-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9DCCB2-1B1E-4A53-9321-62997582A8A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30321E70-A60C-49E6-9C6E-C47D639B7351}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Customer Name</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>{bookings:eng_name}</t>
+  </si>
+  <si>
+    <t>Booking Create Date</t>
+  </si>
+  <si>
+    <t>{bookings:create_date}</t>
   </si>
 </sst>
 </file>
@@ -524,34 +530,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
-    <col min="4" max="4" width="25.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.21875" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="20.5546875" customWidth="1"/>
-    <col min="12" max="12" width="34.5546875" customWidth="1"/>
-    <col min="13" max="13" width="20.88671875" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
-    <col min="15" max="15" width="24.44140625" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" customWidth="1"/>
-    <col min="17" max="17" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="24.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -559,58 +565,61 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -618,54 +627,57 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>